<commit_message>
Ready to bulk test 1,5,10,50
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="98">
   <si>
     <t>4Store_1</t>
   </si>
@@ -323,14 +323,14 @@
     <t xml:space="preserve">7.6 GB </t>
   </si>
   <si>
-    <t>Average Time Fulltext</t>
+    <t>Average regex Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +393,12 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="CMR9"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -494,7 +500,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="321">
+  <cellStyleXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -816,8 +822,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -854,8 +862,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="321">
+  <cellStyles count="323">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1016,6 +1027,7 @@
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1176,6 +1188,7 @@
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2995,7 +3008,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.950348303877522"/>
+          <c:y val="0.257306182648619"/>
+          <c:w val="0.0496516961224777"/>
+          <c:h val="0.485387634702762"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7189,8 +7211,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>141</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -20864,8 +20886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:BG427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB110" workbookViewId="0">
-      <selection activeCell="AQ124" sqref="AQ124"/>
+    <sheetView tabSelected="1" topLeftCell="Y116" workbookViewId="0">
+      <selection activeCell="AF139" sqref="AF139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21664,7 +21686,7 @@
       <c r="AI12" s="3">
         <v>40</v>
       </c>
-      <c r="AJ12" s="4">
+      <c r="AJ12" s="20">
         <v>-3</v>
       </c>
       <c r="AK12" s="3">
@@ -21781,7 +21803,7 @@
       <c r="AI13" s="3">
         <v>1013</v>
       </c>
-      <c r="AJ13" s="4">
+      <c r="AJ13" s="20">
         <v>-3</v>
       </c>
       <c r="AK13" s="3">
@@ -21910,7 +21932,7 @@
       <c r="AI14" s="3">
         <v>40</v>
       </c>
-      <c r="AJ14" s="4">
+      <c r="AJ14" s="20">
         <v>-3</v>
       </c>
       <c r="AK14" s="3">
@@ -22027,7 +22049,7 @@
       <c r="AI15" s="3">
         <v>1013</v>
       </c>
-      <c r="AJ15" s="4">
+      <c r="AJ15" s="20">
         <v>-3</v>
       </c>
       <c r="AK15" s="3">
@@ -22156,7 +22178,7 @@
       <c r="AI16" s="3">
         <v>1031</v>
       </c>
-      <c r="AJ16" s="4">
+      <c r="AJ16" s="20">
         <v>-3</v>
       </c>
       <c r="AK16" s="3">
@@ -22273,7 +22295,7 @@
       <c r="AI17" s="3">
         <v>3</v>
       </c>
-      <c r="AJ17" s="4">
+      <c r="AJ17" s="20">
         <v>-3</v>
       </c>
       <c r="AK17" s="3">
@@ -22402,7 +22424,7 @@
       <c r="AI18" s="3">
         <v>95</v>
       </c>
-      <c r="AJ18" s="4">
+      <c r="AJ18" s="20">
         <v>-3</v>
       </c>
       <c r="AK18" s="3">
@@ -22519,7 +22541,7 @@
       <c r="AI19" s="3">
         <v>95</v>
       </c>
-      <c r="AJ19" s="4">
+      <c r="AJ19" s="20">
         <v>-3</v>
       </c>
       <c r="AK19" s="3">
@@ -22648,7 +22670,7 @@
       <c r="AI20" s="3">
         <v>40</v>
       </c>
-      <c r="AJ20" s="4">
+      <c r="AJ20" s="20">
         <v>-3</v>
       </c>
       <c r="AK20" s="3">
@@ -22765,7 +22787,7 @@
       <c r="AI21" s="3">
         <v>40</v>
       </c>
-      <c r="AJ21" s="4">
+      <c r="AJ21" s="20">
         <v>-3</v>
       </c>
       <c r="AK21" s="3">
@@ -22876,7 +22898,7 @@
       <c r="AI22" s="3">
         <v>14</v>
       </c>
-      <c r="AJ22" s="4">
+      <c r="AJ22" s="20">
         <v>-3</v>
       </c>
       <c r="AK22" s="3">
@@ -22987,7 +23009,7 @@
       <c r="AI23" s="3">
         <v>0</v>
       </c>
-      <c r="AJ23" s="4">
+      <c r="AJ23" s="20">
         <v>-3</v>
       </c>
       <c r="AK23" s="3">
@@ -23098,7 +23120,7 @@
       <c r="AI24" s="3">
         <v>123</v>
       </c>
-      <c r="AJ24" s="4">
+      <c r="AJ24" s="20">
         <v>-3</v>
       </c>
       <c r="AK24" s="3">
@@ -23130,7 +23152,7 @@
       <c r="AI25" s="3">
         <v>0</v>
       </c>
-      <c r="AJ25" s="4">
+      <c r="AJ25" s="20">
         <v>-3</v>
       </c>
       <c r="AK25" s="3">
@@ -23162,7 +23184,7 @@
       <c r="AI26" s="3">
         <v>22</v>
       </c>
-      <c r="AJ26" s="4">
+      <c r="AJ26" s="20">
         <v>-3</v>
       </c>
       <c r="AK26" s="3">
@@ -23191,10 +23213,10 @@
       <c r="AH27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AI27" s="4">
+      <c r="AI27" s="20">
         <v>-3</v>
       </c>
-      <c r="AJ27" s="4">
+      <c r="AJ27" s="20">
         <v>-3</v>
       </c>
       <c r="AK27" s="3">
@@ -23223,10 +23245,10 @@
       <c r="AH28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AI28" s="4">
+      <c r="AI28" s="20">
         <v>-3</v>
       </c>
-      <c r="AJ28" s="4">
+      <c r="AJ28" s="20">
         <v>-3</v>
       </c>
       <c r="AK28" s="3">
@@ -23244,10 +23266,10 @@
       <c r="AO28" s="3">
         <v>14</v>
       </c>
-      <c r="AP28" s="4">
+      <c r="AP28" s="20">
         <v>16</v>
       </c>
-      <c r="AQ28" s="4">
+      <c r="AQ28" s="20">
         <v>16</v>
       </c>
     </row>
@@ -23255,10 +23277,10 @@
       <c r="AH29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AI29" s="4">
+      <c r="AI29" s="20">
         <v>954</v>
       </c>
-      <c r="AJ29" s="4">
+      <c r="AJ29" s="20">
         <v>-3</v>
       </c>
       <c r="AK29" s="3">
@@ -23276,10 +23298,10 @@
       <c r="AO29" s="3">
         <v>939</v>
       </c>
-      <c r="AP29" s="4">
-        <v>40</v>
-      </c>
-      <c r="AQ29" s="4">
+      <c r="AP29" s="20">
+        <v>40</v>
+      </c>
+      <c r="AQ29" s="20">
         <v>40</v>
       </c>
     </row>
@@ -23318,10 +23340,10 @@
       <c r="AH30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AI30" s="4">
+      <c r="AI30" s="20">
         <v>-3</v>
       </c>
-      <c r="AJ30" s="4">
+      <c r="AJ30" s="20">
         <v>-3</v>
       </c>
       <c r="AK30" s="3">
@@ -23339,10 +23361,10 @@
       <c r="AO30" s="3">
         <v>32</v>
       </c>
-      <c r="AP30" s="4">
+      <c r="AP30" s="20">
         <v>939</v>
       </c>
-      <c r="AQ30" s="4">
+      <c r="AQ30" s="20">
         <v>939</v>
       </c>
     </row>
@@ -23389,10 +23411,10 @@
       <c r="AH31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AI31" s="4">
+      <c r="AI31" s="20">
         <v>-3</v>
       </c>
-      <c r="AJ31" s="4">
+      <c r="AJ31" s="20">
         <v>-3</v>
       </c>
       <c r="AK31" s="3">
@@ -23410,10 +23432,10 @@
       <c r="AO31" s="3">
         <v>71</v>
       </c>
-      <c r="AP31" s="4">
+      <c r="AP31" s="20">
         <v>-3</v>
       </c>
-      <c r="AQ31" s="4">
+      <c r="AQ31" s="20">
         <v>-3</v>
       </c>
     </row>
@@ -23503,7 +23525,7 @@
       <c r="AI32" s="3">
         <v>40</v>
       </c>
-      <c r="AJ32" s="4">
+      <c r="AJ32" s="20">
         <v>-3</v>
       </c>
       <c r="AK32" s="3">
@@ -23611,19 +23633,19 @@
       <c r="AH33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AI33" s="4">
+      <c r="AI33" s="20">
         <v>-3</v>
       </c>
-      <c r="AJ33" s="4">
+      <c r="AJ33" s="20">
         <v>-3</v>
       </c>
-      <c r="AK33" s="4">
+      <c r="AK33" s="20">
         <v>-3</v>
       </c>
-      <c r="AL33" s="6">
+      <c r="AL33" s="21">
         <v>-3</v>
       </c>
-      <c r="AM33" s="4">
+      <c r="AM33" s="20">
         <v>-3</v>
       </c>
       <c r="AN33" s="3">
@@ -23632,10 +23654,10 @@
       <c r="AO33" s="3">
         <v>40</v>
       </c>
-      <c r="AP33" s="4">
+      <c r="AP33" s="20">
         <v>-3</v>
       </c>
-      <c r="AQ33" s="4">
+      <c r="AQ33" s="20">
         <v>-3</v>
       </c>
     </row>
@@ -23725,7 +23747,7 @@
       <c r="AI34" s="3">
         <v>10</v>
       </c>
-      <c r="AJ34" s="4">
+      <c r="AJ34" s="20">
         <v>-3</v>
       </c>
       <c r="AK34" s="3">
@@ -23737,10 +23759,10 @@
       <c r="AM34" s="3">
         <v>10</v>
       </c>
-      <c r="AN34" s="4">
+      <c r="AN34" s="20">
         <v>1013</v>
       </c>
-      <c r="AO34" s="4">
+      <c r="AO34" s="20">
         <v>1013</v>
       </c>
       <c r="AP34" s="3">
@@ -23836,7 +23858,7 @@
       <c r="AI35" s="3">
         <v>1013</v>
       </c>
-      <c r="AJ35" s="4">
+      <c r="AJ35" s="20">
         <v>-3</v>
       </c>
       <c r="AK35" s="3">
@@ -37429,15 +37451,42 @@
         <v>97</v>
       </c>
       <c r="AH166" s="17"/>
-      <c r="AI166" s="17"/>
-      <c r="AJ166" s="17"/>
-      <c r="AK166" s="17"/>
-      <c r="AL166" s="17"/>
-      <c r="AM166" s="17"/>
-      <c r="AN166" s="17"/>
-      <c r="AO166" s="17"/>
-      <c r="AP166" s="17"/>
-      <c r="AQ166" s="17"/>
+      <c r="AI166" s="17">
+        <f>AVERAGE(AI146:AI165)</f>
+        <v>5661.6842105263158</v>
+      </c>
+      <c r="AJ166" s="17">
+        <f t="shared" ref="AJ166:AQ166" si="0">AVERAGE(AJ146:AJ165)</f>
+        <v>3326.8421052631579</v>
+      </c>
+      <c r="AK166" s="17">
+        <f t="shared" si="0"/>
+        <v>19145.473684210527</v>
+      </c>
+      <c r="AL166" s="17">
+        <f t="shared" si="0"/>
+        <v>1083.2105263157894</v>
+      </c>
+      <c r="AM166" s="17">
+        <f t="shared" si="0"/>
+        <v>1342.7368421052631</v>
+      </c>
+      <c r="AN166" s="17">
+        <f t="shared" si="0"/>
+        <v>972.9473684210526</v>
+      </c>
+      <c r="AO166" s="17">
+        <f t="shared" si="0"/>
+        <v>2249.9473684210525</v>
+      </c>
+      <c r="AP166" s="17">
+        <f t="shared" si="0"/>
+        <v>31189.684210526317</v>
+      </c>
+      <c r="AQ166" s="17">
+        <f t="shared" si="0"/>
+        <v>1046.2631578947369</v>
+      </c>
       <c r="AR166" s="17"/>
       <c r="AS166" s="17"/>
       <c r="AT166" s="17"/>
@@ -43922,17 +43971,46 @@
       <c r="AC225" s="1">
         <v>5855</v>
       </c>
-      <c r="AG225" s="17"/>
+      <c r="AG225" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="AH225" s="17"/>
-      <c r="AI225" s="17"/>
-      <c r="AJ225" s="17"/>
-      <c r="AK225" s="17"/>
-      <c r="AL225" s="17"/>
-      <c r="AM225" s="17"/>
-      <c r="AN225" s="17"/>
-      <c r="AO225" s="17"/>
-      <c r="AP225" s="17"/>
-      <c r="AQ225" s="17"/>
+      <c r="AI225" s="17">
+        <f>AVERAGE(AVERAGE(AI205:AI224))</f>
+        <v>111101.26315789473</v>
+      </c>
+      <c r="AJ225" s="17">
+        <f t="shared" ref="AJ225:AQ225" si="1">AVERAGE(AVERAGE(AJ205:AJ224))</f>
+        <v>27834.36842105263</v>
+      </c>
+      <c r="AK225" s="17">
+        <f t="shared" si="1"/>
+        <v>15141.947368421053</v>
+      </c>
+      <c r="AL225" s="17">
+        <f t="shared" si="1"/>
+        <v>2822.1052631578946</v>
+      </c>
+      <c r="AM225" s="17">
+        <f t="shared" si="1"/>
+        <v>5587.0526315789475</v>
+      </c>
+      <c r="AN225" s="17">
+        <f t="shared" si="1"/>
+        <v>5487.6842105263158</v>
+      </c>
+      <c r="AO225" s="17">
+        <f t="shared" si="1"/>
+        <v>6489.894736842105</v>
+      </c>
+      <c r="AP225" s="17">
+        <f t="shared" si="1"/>
+        <v>163081.63157894736</v>
+      </c>
+      <c r="AQ225" s="17">
+        <f t="shared" si="1"/>
+        <v>5127.7894736842109</v>
+      </c>
       <c r="AR225" s="17"/>
       <c r="AS225" s="17"/>
       <c r="AT225" s="17"/>
@@ -44697,7 +44775,7 @@
       <c r="AI238" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AJ238" s="17">
+      <c r="AJ238" s="22">
         <v>12</v>
       </c>
       <c r="AK238" s="17"/>
@@ -44793,7 +44871,7 @@
       <c r="AI239" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="AJ239" s="17">
+      <c r="AJ239" s="22">
         <v>15</v>
       </c>
       <c r="AK239" s="17"/>
@@ -44889,7 +44967,7 @@
       <c r="AI240" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="AJ240" s="17">
+      <c r="AJ240" s="22">
         <v>33</v>
       </c>
       <c r="AK240" s="17"/>
@@ -44985,7 +45063,7 @@
       <c r="AI241" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AJ241" s="17">
+      <c r="AJ241" s="22">
         <v>19</v>
       </c>
       <c r="AK241" s="17"/>
@@ -45081,7 +45159,7 @@
       <c r="AI242" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AJ242" s="17">
+      <c r="AJ242" s="22">
         <v>13</v>
       </c>
       <c r="AK242" s="17"/>
@@ -45177,7 +45255,7 @@
       <c r="AI243" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AJ243" s="17">
+      <c r="AJ243" s="22">
         <v>14</v>
       </c>
       <c r="AK243" s="17"/>
@@ -45273,7 +45351,7 @@
       <c r="AI244" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="AJ244" s="17">
+      <c r="AJ244" s="22">
         <v>5</v>
       </c>
       <c r="AK244" s="17"/>
@@ -45369,7 +45447,7 @@
       <c r="AI245" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="AJ245" s="17">
+      <c r="AJ245" s="22">
         <v>66</v>
       </c>
       <c r="AK245" s="17"/>
@@ -45465,7 +45543,7 @@
       <c r="AI246" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="AJ246" s="17">
+      <c r="AJ246" s="22">
         <v>92</v>
       </c>
       <c r="AK246" s="17"/>

</xml_diff>